<commit_message>
Tweaked wall positions of area 2. SHould be finished now
</commit_message>
<xml_diff>
--- a/LabyrinthExplorer/area2.xlsx
+++ b/LabyrinthExplorer/area2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="13">
   <si>
     <t>x1</t>
   </si>
@@ -38,12 +38,30 @@
   <si>
     <t>,</t>
   </si>
+  <si>
+    <t>//bottom left middle wall</t>
+  </si>
+  <si>
+    <t>//move down 50</t>
+  </si>
+  <si>
+    <t>//pillar 2 botttom corner</t>
+  </si>
+  <si>
+    <t>///wall right of above wall</t>
+  </si>
+  <si>
+    <t>//move 50 down</t>
+  </si>
+  <si>
+    <t>move 50 down</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,13 +85,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,19 +127,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -393,8 +442,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J68" sqref="A68:J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -407,7 +456,7 @@
     <col min="6" max="6" width="16.140625" customWidth="1"/>
     <col min="7" max="7" width="1.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="34.5" customHeight="1">
@@ -483,19 +532,19 @@
         <v>6</v>
       </c>
       <c r="D3" s="3">
-        <v>900</v>
+        <v>50</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="3">
-        <v>850</v>
+        <v>4950</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="3">
-        <v>900</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s">
         <v>5</v>
@@ -528,19 +577,19 @@
         <v>6</v>
       </c>
       <c r="D4" s="3">
-        <v>50</v>
+        <v>900</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="3">
-        <v>4950</v>
+        <v>850</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="3">
-        <v>50</v>
+        <v>900</v>
       </c>
       <c r="I4" t="s">
         <v>5</v>
@@ -618,19 +667,19 @@
         <v>6</v>
       </c>
       <c r="D6" s="3">
-        <v>2550</v>
+        <v>1700</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="3">
-        <v>350</v>
+        <v>1450</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="3">
-        <v>1500</v>
+        <v>1700</v>
       </c>
       <c r="I6" t="s">
         <v>5</v>
@@ -663,7 +712,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="3">
-        <v>3800</v>
+        <v>2550</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>6</v>
@@ -675,7 +724,7 @@
         <v>6</v>
       </c>
       <c r="H7" s="3">
-        <v>2900</v>
+        <v>1500</v>
       </c>
       <c r="I7" t="s">
         <v>5</v>
@@ -708,7 +757,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="3">
-        <v>4750</v>
+        <v>3800</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>6</v>
@@ -720,7 +769,7 @@
         <v>6</v>
       </c>
       <c r="H8" s="3">
-        <v>4150</v>
+        <v>2900</v>
       </c>
       <c r="I8" t="s">
         <v>5</v>
@@ -753,19 +802,19 @@
         <v>6</v>
       </c>
       <c r="D9" s="3">
-        <v>1700</v>
+        <v>4750</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="3">
-        <v>1450</v>
+        <v>350</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H9" s="3">
-        <v>1700</v>
+        <v>4150</v>
       </c>
       <c r="I9" t="s">
         <v>5</v>
@@ -788,34 +837,36 @@
       </c>
     </row>
     <row r="10" spans="1:25" s="2" customFormat="1">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3">
+      <c r="A10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7">
         <v>650</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="C10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="7">
         <v>2250</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="E10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="7">
         <v>650</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="3">
+      <c r="G10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="7">
         <v>2600</v>
       </c>
-      <c r="I10" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10"/>
+      <c r="I10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="K10"/>
       <c r="L10"/>
       <c r="M10"/>
@@ -923,34 +974,36 @@
       </c>
     </row>
     <row r="13" spans="1:25" s="2" customFormat="1">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3">
+      <c r="A13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="7">
         <v>1050</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="C13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="7">
         <v>3750</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="E13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="7">
         <v>1050</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="G13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="7">
         <v>2900</v>
       </c>
-      <c r="I13" t="s">
-        <v>5</v>
-      </c>
-      <c r="J13"/>
+      <c r="I13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="K13"/>
       <c r="L13"/>
       <c r="M13"/>
@@ -978,19 +1031,19 @@
         <v>6</v>
       </c>
       <c r="D14" s="3">
-        <v>4750</v>
+        <v>4450</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="3">
-        <v>350</v>
+        <v>2000</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="3">
-        <v>4750</v>
+        <v>4450</v>
       </c>
       <c r="I14" t="s">
         <v>5</v>
@@ -1023,19 +1076,19 @@
         <v>6</v>
       </c>
       <c r="D15" s="3">
-        <v>4950</v>
+        <v>4750</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="3">
-        <v>1250</v>
+        <v>350</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H15" s="3">
-        <v>4450</v>
+        <v>4750</v>
       </c>
       <c r="I15" t="s">
         <v>5</v>
@@ -1058,34 +1111,36 @@
       </c>
     </row>
     <row r="16" spans="1:25" s="2" customFormat="1">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="3">
+      <c r="A16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="7">
         <v>1250</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="3">
+      <c r="C16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="7">
+        <v>4950</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="7">
+        <v>1250</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="7">
         <v>4450</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="3">
-        <v>2000</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="3">
-        <v>4450</v>
-      </c>
-      <c r="I16" t="s">
-        <v>5</v>
-      </c>
-      <c r="J16"/>
+      <c r="I16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="K16"/>
       <c r="L16"/>
       <c r="M16"/>
@@ -1293,19 +1348,19 @@
         <v>6</v>
       </c>
       <c r="D21" s="3">
-        <v>2900</v>
+        <v>2600</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F21" s="3">
-        <v>650</v>
+        <v>1450</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H21" s="3">
-        <v>2900</v>
+        <v>1700</v>
       </c>
       <c r="I21" t="s">
         <v>5</v>
@@ -1338,19 +1393,19 @@
         <v>6</v>
       </c>
       <c r="D22" s="3">
-        <v>2600</v>
+        <v>2900</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F22" s="3">
-        <v>1450</v>
+        <v>650</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H22" s="3">
-        <v>1700</v>
+        <v>2900</v>
       </c>
       <c r="I22" t="s">
         <v>5</v>
@@ -1418,34 +1473,36 @@
       </c>
     </row>
     <row r="24" spans="1:25" s="2" customFormat="1">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3">
+      <c r="A24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="7">
         <v>1700</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="3">
+      <c r="C24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="7">
         <v>2150</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="3">
+      <c r="E24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="7">
         <v>1700</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" s="3">
+      <c r="G24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="7">
         <v>2600</v>
       </c>
-      <c r="I24" t="s">
-        <v>5</v>
-      </c>
-      <c r="J24"/>
+      <c r="I24" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="K24"/>
       <c r="L24"/>
       <c r="M24"/>
@@ -1508,34 +1565,36 @@
       </c>
     </row>
     <row r="26" spans="1:25" s="2" customFormat="1">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="3">
+      <c r="A26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="7">
         <v>1700</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="3">
+      <c r="C26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="7">
         <v>3600</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="3">
+      <c r="E26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="7">
         <v>1700</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="3">
+      <c r="G26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="7">
         <v>3950</v>
       </c>
-      <c r="I26" t="s">
-        <v>5</v>
-      </c>
-      <c r="J26"/>
+      <c r="I26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="K26"/>
       <c r="L26"/>
       <c r="M26"/>
@@ -1653,13 +1712,13 @@
         <v>6</v>
       </c>
       <c r="D29" s="3">
-        <v>900</v>
+        <v>400</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F29" s="3">
-        <v>1300</v>
+        <v>2050</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>6</v>
@@ -1698,13 +1757,13 @@
         <v>6</v>
       </c>
       <c r="D30" s="3">
-        <v>400</v>
+        <v>900</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F30" s="3">
-        <v>2050</v>
+        <v>1300</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>6</v>
@@ -1777,7 +1836,7 @@
         <v>24450</v>
       </c>
     </row>
-    <row r="32" spans="1:25" s="2" customFormat="1">
+    <row r="32" spans="1:25" s="2" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1867,7 +1926,7 @@
         <v>24750</v>
       </c>
     </row>
-    <row r="34" spans="1:25" s="2" customFormat="1">
+    <row r="34" spans="1:25" s="2" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1913,34 +1972,36 @@
       </c>
     </row>
     <row r="35" spans="1:25" s="2" customFormat="1">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="3">
+      <c r="A35" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="7">
         <v>2350</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="3">
-        <v>4650</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" s="3">
-        <v>1400</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H35" s="3">
-        <v>4650</v>
-      </c>
-      <c r="I35" t="s">
-        <v>5</v>
-      </c>
-      <c r="J35"/>
+      <c r="C35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="6">
+        <v>200</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="7">
+        <v>2350</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="7">
+        <v>950</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="K35"/>
       <c r="L35"/>
       <c r="M35"/>
@@ -1967,8 +2028,8 @@
       <c r="C36" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="2">
-        <v>200</v>
+      <c r="D36" s="3">
+        <v>3600</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>6</v>
@@ -1980,12 +2041,14 @@
         <v>6</v>
       </c>
       <c r="H36" s="3">
-        <v>950</v>
+        <v>4650</v>
       </c>
       <c r="I36" t="s">
         <v>5</v>
       </c>
-      <c r="J36"/>
+      <c r="J36" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="K36"/>
       <c r="L36"/>
       <c r="M36"/>
@@ -2013,13 +2076,13 @@
         <v>6</v>
       </c>
       <c r="D37" s="3">
-        <v>3600</v>
+        <v>4650</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F37" s="3">
-        <v>2350</v>
+        <v>1400</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>6</v>
@@ -2030,7 +2093,9 @@
       <c r="I37" t="s">
         <v>5</v>
       </c>
-      <c r="J37"/>
+      <c r="J37" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="K37"/>
       <c r="L37"/>
       <c r="M37"/>
@@ -2093,34 +2158,36 @@
       </c>
     </row>
     <row r="39" spans="1:25" s="2" customFormat="1">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="3">
+      <c r="A39" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="7">
         <v>2400</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="3">
+      <c r="C39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="7">
         <v>1200</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" s="3">
+      <c r="E39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="7">
         <v>2400</v>
       </c>
-      <c r="G39" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H39" s="3">
+      <c r="G39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="7">
         <v>1600</v>
       </c>
-      <c r="I39" t="s">
-        <v>5</v>
-      </c>
-      <c r="J39"/>
+      <c r="I39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="K39"/>
       <c r="L39"/>
       <c r="M39"/>
@@ -2165,7 +2232,9 @@
       <c r="I40" t="s">
         <v>5</v>
       </c>
-      <c r="J40"/>
+      <c r="J40" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="K40"/>
       <c r="L40"/>
       <c r="M40"/>
@@ -2183,34 +2252,36 @@
       </c>
     </row>
     <row r="41" spans="1:25" s="2" customFormat="1">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="3">
+      <c r="A41" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="7">
         <v>2650</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="3">
+      <c r="C41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="7">
         <v>3800</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="3">
+      <c r="E41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="7">
         <v>2650</v>
       </c>
-      <c r="G41" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H41" s="3">
+      <c r="G41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="7">
         <v>4100</v>
       </c>
-      <c r="I41" t="s">
-        <v>5</v>
-      </c>
-      <c r="J41"/>
+      <c r="I41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="K41"/>
       <c r="L41"/>
       <c r="M41"/>
@@ -2238,19 +2309,19 @@
         <v>6</v>
       </c>
       <c r="D42" s="3">
-        <v>4300</v>
+        <v>4100</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F42" s="3">
-        <v>2650</v>
+        <v>3350</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H42" s="3">
-        <v>4650</v>
+        <v>4100</v>
       </c>
       <c r="I42" t="s">
         <v>5</v>
@@ -2283,19 +2354,19 @@
         <v>6</v>
       </c>
       <c r="D43" s="3">
-        <v>4100</v>
+        <v>4300</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F43" s="3">
-        <v>3350</v>
+        <v>2650</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H43" s="3">
-        <v>4100</v>
+        <v>4650</v>
       </c>
       <c r="I43" t="s">
         <v>5</v>
@@ -2373,19 +2444,19 @@
         <v>6</v>
       </c>
       <c r="D45" s="3">
-        <v>3350</v>
+        <v>2150</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F45" s="3">
+        <v>3100</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="3">
         <v>2600</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H45" s="3">
-        <v>3350</v>
       </c>
       <c r="I45" t="s">
         <v>5</v>
@@ -2418,13 +2489,13 @@
         <v>6</v>
       </c>
       <c r="D46" s="3">
-        <v>2150</v>
+        <v>2600</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F46" s="3">
-        <v>3100</v>
+        <v>4600</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>6</v>
@@ -2553,19 +2624,19 @@
         <v>6</v>
       </c>
       <c r="D49" s="3">
+        <v>3350</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="3">
         <v>2600</v>
       </c>
-      <c r="E49" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F49" s="3">
-        <v>4600</v>
-      </c>
       <c r="G49" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H49" s="3">
-        <v>2600</v>
+        <v>3350</v>
       </c>
       <c r="I49" t="s">
         <v>5</v>
@@ -2598,19 +2669,19 @@
         <v>6</v>
       </c>
       <c r="D50" s="3">
-        <v>3800</v>
+        <v>2900</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F50" s="3">
-        <v>2650</v>
+        <v>3350</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H50" s="3">
-        <v>3800</v>
+        <v>4100</v>
       </c>
       <c r="I50" t="s">
         <v>5</v>
@@ -2643,19 +2714,19 @@
         <v>6</v>
       </c>
       <c r="D51" s="3">
-        <v>2900</v>
+        <v>3800</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F51" s="3">
-        <v>3350</v>
+        <v>2650</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H51" s="3">
-        <v>4100</v>
+        <v>3800</v>
       </c>
       <c r="I51" t="s">
         <v>5</v>
@@ -2823,19 +2894,19 @@
         <v>6</v>
       </c>
       <c r="D55" s="3">
-        <v>3800</v>
+        <v>2900</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F55" s="3">
-        <v>3650</v>
+        <v>4600</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H55" s="3">
-        <v>4300</v>
+        <v>2900</v>
       </c>
       <c r="I55" t="s">
         <v>5</v>
@@ -2868,19 +2939,19 @@
         <v>6</v>
       </c>
       <c r="D56" s="3">
-        <v>2900</v>
+        <v>3800</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F56" s="3">
-        <v>4600</v>
+        <v>3650</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H56" s="3">
-        <v>2900</v>
+        <v>4300</v>
       </c>
       <c r="I56" t="s">
         <v>5</v>
@@ -2958,13 +3029,13 @@
         <v>6</v>
       </c>
       <c r="D58" s="3">
-        <v>3300</v>
+        <v>3100</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F58" s="3">
-        <v>3900</v>
+        <v>4300</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>6</v>
@@ -3003,7 +3074,7 @@
         <v>6</v>
       </c>
       <c r="D59" s="3">
-        <v>3500</v>
+        <v>3300</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>6</v>
@@ -3015,7 +3086,7 @@
         <v>6</v>
       </c>
       <c r="H59" s="3">
-        <v>4100</v>
+        <v>3100</v>
       </c>
       <c r="I59" t="s">
         <v>5</v>
@@ -3048,19 +3119,19 @@
         <v>6</v>
       </c>
       <c r="D60" s="3">
-        <v>4100</v>
+        <v>3300</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F60" s="3">
-        <v>4100</v>
+        <v>4300</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H60" s="3">
-        <v>4100</v>
+        <v>3300</v>
       </c>
       <c r="I60" t="s">
         <v>5</v>
@@ -3099,13 +3170,13 @@
         <v>6</v>
       </c>
       <c r="F61" s="3">
-        <v>4150</v>
+        <v>3900</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H61" s="3">
-        <v>3500</v>
+        <v>4100</v>
       </c>
       <c r="I61" t="s">
         <v>5</v>
@@ -3138,19 +3209,19 @@
         <v>6</v>
       </c>
       <c r="D62" s="3">
-        <v>3650</v>
+        <v>3500</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F62" s="3">
-        <v>4250</v>
+        <v>4150</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H62" s="3">
-        <v>3650</v>
+        <v>3500</v>
       </c>
       <c r="I62" t="s">
         <v>5</v>
@@ -3183,19 +3254,19 @@
         <v>6</v>
       </c>
       <c r="D63" s="3">
-        <v>3100</v>
+        <v>3650</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F63" s="3">
-        <v>4300</v>
+        <v>4250</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H63" s="3">
-        <v>3100</v>
+        <v>3650</v>
       </c>
       <c r="I63" t="s">
         <v>5</v>
@@ -3228,19 +3299,19 @@
         <v>6</v>
       </c>
       <c r="D64" s="3">
-        <v>3300</v>
+        <v>4100</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F64" s="3">
-        <v>4300</v>
+        <v>4100</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H64" s="3">
-        <v>3300</v>
+        <v>4100</v>
       </c>
       <c r="I64" t="s">
         <v>5</v>
@@ -3307,48 +3378,47 @@
         <v>23450</v>
       </c>
     </row>
-    <row r="66" spans="1:25" s="2" customFormat="1">
-      <c r="A66" t="s">
-        <v>4</v>
-      </c>
-      <c r="B66" s="3">
+    <row r="66" spans="1:25" s="6" customFormat="1">
+      <c r="A66" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="7">
         <v>4250</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D66" s="3">
+      <c r="C66" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="7">
         <v>950</v>
       </c>
-      <c r="E66" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F66" s="3">
+      <c r="E66" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66" s="7">
         <v>4250</v>
       </c>
-      <c r="G66" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H66" s="3">
+      <c r="G66" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H66" s="7">
         <v>1650</v>
       </c>
-      <c r="I66" t="s">
-        <v>5</v>
-      </c>
-      <c r="J66"/>
-      <c r="K66"/>
-      <c r="L66"/>
-      <c r="M66"/>
-      <c r="V66" s="2">
+      <c r="I66" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V66" s="6">
         <v>13450</v>
       </c>
-      <c r="W66" s="2">
+      <c r="W66" s="6">
         <v>11950</v>
       </c>
-      <c r="X66" s="2">
+      <c r="X66" s="6">
         <v>24950</v>
       </c>
-      <c r="Y66" s="2">
+      <c r="Y66" s="6">
         <v>21950</v>
       </c>
     </row>
@@ -3363,19 +3433,19 @@
         <v>6</v>
       </c>
       <c r="D67" s="3">
-        <v>3300</v>
+        <v>1650</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F67" s="3">
-        <v>4250</v>
+        <v>4700</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H67" s="3">
-        <v>3650</v>
+        <v>1650</v>
       </c>
       <c r="I67" t="s">
         <v>5</v>
@@ -3398,34 +3468,36 @@
       </c>
     </row>
     <row r="68" spans="1:25" s="2" customFormat="1">
-      <c r="A68" t="s">
-        <v>4</v>
-      </c>
-      <c r="B68" s="3">
+      <c r="A68" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="7">
         <v>4250</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="3">
-        <v>1650</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F68" s="3">
-        <v>4700</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H68" s="3">
-        <v>1650</v>
-      </c>
-      <c r="I68" t="s">
-        <v>5</v>
-      </c>
-      <c r="J68"/>
+      <c r="C68" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="7">
+        <v>3300</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F68" s="7">
+        <v>4250</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H68" s="7">
+        <v>3650</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J68" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="K68"/>
       <c r="L68"/>
       <c r="M68"/>
@@ -3453,19 +3525,19 @@
         <v>6</v>
       </c>
       <c r="D69" s="3">
-        <v>4100</v>
+        <v>3300</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F69" s="3">
-        <v>4300</v>
+        <v>4600</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H69" s="3">
-        <v>3800</v>
+        <v>3300</v>
       </c>
       <c r="I69" t="s">
         <v>5</v>
@@ -3498,24 +3570,26 @@
         <v>6</v>
       </c>
       <c r="D70" s="3">
-        <v>3300</v>
+        <v>4100</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F70" s="3">
-        <v>4600</v>
+        <v>4300</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H70" s="3">
-        <v>3300</v>
+        <v>3800</v>
       </c>
       <c r="I70" t="s">
         <v>5</v>
       </c>
-      <c r="J70"/>
+      <c r="J70" t="s">
+        <v>11</v>
+      </c>
       <c r="K70"/>
       <c r="L70"/>
       <c r="M70"/>
@@ -3848,11 +3922,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:H77">
+  <sortState ref="A2:I77">
     <sortCondition ref="B2:B77"/>
-    <sortCondition ref="F2:F77"/>
     <sortCondition ref="D2:D77"/>
-    <sortCondition ref="H2:H77"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>